<commit_message>
updates for main file
</commit_message>
<xml_diff>
--- a/FIFA.xlsx
+++ b/FIFA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modri\IH-labs\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8606EC9A-05FD-4F65-A9C5-B6E671C634A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F675AE3F-6756-4B24-8D38-D5A518830E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C125" sqref="C125"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1813,6 +1813,9 @@
       <c r="B90">
         <v>229</v>
       </c>
+      <c r="C90">
+        <v>146900</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">

</xml_diff>